<commit_message>
add modifications to MLs
</commit_message>
<xml_diff>
--- a/top9_outlier.xlsx
+++ b/top9_outlier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -46,61 +46,61 @@
     <t>bt_error</t>
   </si>
   <si>
+    <t>Co(Cp-op-Ph(CH₃)₃)(Cp-op-Ph(CH₃)₃)OH</t>
+  </si>
+  <si>
+    <t>Co(Cp-(CO)NH₂)(Cp-p-PhOCH₃)OH</t>
+  </si>
+  <si>
     <t>Co(Cp-P(CH₃)₂)(Cp-(CO)NH₂)OH</t>
   </si>
   <si>
+    <t>Co(Cp-p-PhCl)(Cp-m-PhCF₃)OH</t>
+  </si>
+  <si>
+    <t>Co(Cp-N(CH₃)₂)(Cp-NC₅H₁₀)OH</t>
+  </si>
+  <si>
     <t>Co(Cp-S(CH₃))(Cp-(CO)NH₂)OH</t>
   </si>
   <si>
-    <t>Co(Cp-(CO)NH₂)(Cp-p-PhOCH₃)OH</t>
-  </si>
-  <si>
-    <t>Co(Cp-op-Ph(CH₃)₃)(Cp-op-Ph(CH₃)₃)OH</t>
-  </si>
-  <si>
     <t>Co(Cp-(CO)NH₂)(Cp-(CO)CH₃)OH</t>
   </si>
   <si>
     <t>Co(Cp-Ph)(Cp-(CO)NH₂)OH</t>
   </si>
   <si>
-    <t>Co(Cp-C₃H₇)(Cp-(CO)NH₂)OH</t>
-  </si>
-  <si>
-    <t>Co(Cp-C₂H₃)(Cp-(CO)NH₂)OH</t>
-  </si>
-  <si>
-    <t>Co(Cp-(CO)NHCH₃)(Cp-(CO)NHCH₃)OH</t>
+    <t>op-Ph(CH₃)₃</t>
   </si>
   <si>
     <t>(CO)NH₂</t>
   </si>
   <si>
-    <t>op-Ph(CH₃)₃</t>
-  </si>
-  <si>
-    <t>(CO)NHCH₃</t>
+    <t>m-PhCF₃</t>
+  </si>
+  <si>
+    <t>N(CH₃)₂</t>
+  </si>
+  <si>
+    <t>p-PhOCH₃</t>
   </si>
   <si>
     <t>P(CH₃)₂</t>
   </si>
   <si>
+    <t>p-PhCl</t>
+  </si>
+  <si>
+    <t>NC₅H₁₀</t>
+  </si>
+  <si>
     <t>S(CH₃)</t>
   </si>
   <si>
-    <t>p-PhOCH₃</t>
-  </si>
-  <si>
     <t>(CO)CH₃</t>
   </si>
   <si>
     <t>Ph</t>
-  </si>
-  <si>
-    <t>C₃H₇</t>
-  </si>
-  <si>
-    <t>C₂H₃</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,42 +498,42 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1">
-        <v>136</v>
+        <v>888</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>18.72200009191488</v>
+        <v>9.139161859725391</v>
       </c>
       <c r="F2">
-        <v>34.29792404174805</v>
+        <v>14.51137542724609</v>
       </c>
       <c r="G2">
-        <v>15.57592394983317</v>
+        <v>5.372213567520703</v>
       </c>
       <c r="H2">
-        <v>32.1035020386832</v>
+        <v>16.13189317495737</v>
       </c>
       <c r="I2">
-        <v>13.38150194676832</v>
+        <v>6.992731315231978</v>
       </c>
       <c r="J2">
-        <v>31.98055000472209</v>
+        <v>15.32765459600909</v>
       </c>
       <c r="K2">
-        <v>13.25854991280721</v>
+        <v>6.188492736283703</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1">
-        <v>174</v>
+        <v>572</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -542,33 +542,33 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
-        <v>32.60614579448315</v>
+        <v>11.55924592858696</v>
       </c>
       <c r="F3">
-        <v>24.37985801696777</v>
+        <v>24.74857902526855</v>
       </c>
       <c r="G3">
-        <v>8.226287777515374</v>
+        <v>13.18933309668159</v>
       </c>
       <c r="H3">
-        <v>25.35923158731025</v>
+        <v>25.82728931886639</v>
       </c>
       <c r="I3">
-        <v>7.246914207172896</v>
+        <v>14.26804339027943</v>
       </c>
       <c r="J3">
-        <v>25.37291332229921</v>
+        <v>24.88187635462293</v>
       </c>
       <c r="K3">
-        <v>7.233232472183936</v>
+        <v>13.32263042603597</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1">
-        <v>572</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -577,33 +577,33 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4">
-        <v>11.55924592858696</v>
+        <v>18.72200009191488</v>
       </c>
       <c r="F4">
-        <v>25.77413368225098</v>
+        <v>34.47745895385742</v>
       </c>
       <c r="G4">
-        <v>14.21488775366402</v>
+        <v>15.75545886194254</v>
       </c>
       <c r="H4">
-        <v>21.49359952248681</v>
+        <v>32.72342214077957</v>
       </c>
       <c r="I4">
-        <v>9.934353593899846</v>
+        <v>14.00142204886469</v>
       </c>
       <c r="J4">
-        <v>25.27532690835394</v>
+        <v>32.92492360318852</v>
       </c>
       <c r="K4">
-        <v>13.71608097976697</v>
+        <v>14.20292351127364</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1">
-        <v>888</v>
+        <v>816</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -612,68 +612,68 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E5">
-        <v>9.139161859725391</v>
+        <v>24.65074768124623</v>
       </c>
       <c r="F5">
-        <v>14.27899837493896</v>
+        <v>28.61704444885254</v>
       </c>
       <c r="G5">
-        <v>5.139836515213574</v>
+        <v>3.966296767606309</v>
       </c>
       <c r="H5">
-        <v>16.10907886487396</v>
+        <v>28.52085478829311</v>
       </c>
       <c r="I5">
-        <v>6.969917005148567</v>
+        <v>3.870107107046877</v>
       </c>
       <c r="J5">
-        <v>16.29385531754929</v>
+        <v>28.71049792510872</v>
       </c>
       <c r="K5">
-        <v>7.154693457823896</v>
+        <v>4.059750243862489</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1">
-        <v>554</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
       <c r="E6">
-        <v>34.91485496414271</v>
+        <v>25.29156945623299</v>
       </c>
       <c r="F6">
-        <v>26.42976188659668</v>
+        <v>20.64176750183105</v>
       </c>
       <c r="G6">
-        <v>8.485093077546033</v>
+        <v>4.649801954401934</v>
       </c>
       <c r="H6">
-        <v>25.44180218496276</v>
+        <v>20.809872202454</v>
       </c>
       <c r="I6">
-        <v>9.473052779179952</v>
+        <v>4.481697253778993</v>
       </c>
       <c r="J6">
-        <v>26.52609735960635</v>
+        <v>20.77560615501056</v>
       </c>
       <c r="K6">
-        <v>8.388757604536359</v>
+        <v>4.515963301222424</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -685,30 +685,30 @@
         <v>26</v>
       </c>
       <c r="E7">
-        <v>35.23320046051026</v>
+        <v>32.60614579448315</v>
       </c>
       <c r="F7">
-        <v>19.68964767456055</v>
+        <v>26.69338989257812</v>
       </c>
       <c r="G7">
-        <v>15.54355278594971</v>
+        <v>5.912755901905022</v>
       </c>
       <c r="H7">
-        <v>17.33454107362625</v>
+        <v>27.25398298025034</v>
       </c>
       <c r="I7">
-        <v>17.89865938688401</v>
+        <v>5.352162814232805</v>
       </c>
       <c r="J7">
-        <v>17.68509571618171</v>
+        <v>21.76100910939113</v>
       </c>
       <c r="K7">
-        <v>17.54810474432855</v>
+        <v>10.84513668509202</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1">
-        <v>381</v>
+        <v>554</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -720,30 +720,30 @@
         <v>27</v>
       </c>
       <c r="E8">
-        <v>41.38571606223763</v>
+        <v>34.91485496414271</v>
       </c>
       <c r="F8">
-        <v>37.23273086547852</v>
+        <v>27.17123985290527</v>
       </c>
       <c r="G8">
-        <v>4.152985196759111</v>
+        <v>7.743615111237439</v>
       </c>
       <c r="H8">
-        <v>31.79646956159659</v>
+        <v>27.29531890579973</v>
       </c>
       <c r="I8">
-        <v>9.589246500641039</v>
+        <v>7.619536058342984</v>
       </c>
       <c r="J8">
-        <v>32.62703537667333</v>
+        <v>26.26056723891668</v>
       </c>
       <c r="K8">
-        <v>8.7586806855643</v>
+        <v>8.654287725226034</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -755,60 +755,25 @@
         <v>28</v>
       </c>
       <c r="E9">
-        <v>33.48385495002276</v>
+        <v>35.23320046051026</v>
       </c>
       <c r="F9">
-        <v>19.75181770324707</v>
+        <v>24.91176414489746</v>
       </c>
       <c r="G9">
-        <v>13.73203724677569</v>
+        <v>10.3214363156128</v>
       </c>
       <c r="H9">
-        <v>16.61664379485658</v>
+        <v>18.97877025140358</v>
       </c>
       <c r="I9">
-        <v>16.86721115516618</v>
+        <v>16.25443020910668</v>
       </c>
       <c r="J9">
-        <v>17.7194620746926</v>
+        <v>17.51388496470531</v>
       </c>
       <c r="K9">
-        <v>15.76439287533016</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1">
-        <v>525</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>12.69772424289272</v>
-      </c>
-      <c r="F10">
-        <v>20.34685707092285</v>
-      </c>
-      <c r="G10">
-        <v>7.649132828030131</v>
-      </c>
-      <c r="H10">
-        <v>19.28421495423549</v>
-      </c>
-      <c r="I10">
-        <v>6.586490711342774</v>
-      </c>
-      <c r="J10">
-        <v>18.80746504960742</v>
-      </c>
-      <c r="K10">
-        <v>6.109740806714699</v>
+        <v>17.71931549580495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>